<commit_message>
feat: Update Drehschwingungen Protokoll
</commit_message>
<xml_diff>
--- a/Physik/Praktikum/Versuch Drehschwingunen/Ergebnisse.xlsx
+++ b/Physik/Praktikum/Versuch Drehschwingunen/Ergebnisse.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/moritz_wieland_bwedu_de/Documents/Module/Physik/Praktikum/Versuch Drehschwingunen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="8_{01A964AD-6641-B540-9A83-878732202AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24727245-330C-5045-A3D9-96DC871243D1}"/>
+  <xr:revisionPtr revIDLastSave="386" documentId="8_{01A964AD-6641-B540-9A83-878732202AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8E06191-5C64-094D-B4FE-07444D263A1F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1DD4A0C7-F59A-A441-B76A-37DAD2FD2B99}"/>
+    <workbookView xWindow="4860" yWindow="22100" windowWidth="28800" windowHeight="17500" xr2:uid="{1DD4A0C7-F59A-A441-B76A-37DAD2FD2B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$F$48:$F$60</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$47</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$H$48:$H$60</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$F$48:$F$60</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$H$47</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$48:$H$60</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,9 +53,6 @@
   </si>
   <si>
     <t>Periodendauer T in s</t>
-  </si>
-  <si>
-    <t>Eigenfrequenz in s</t>
   </si>
   <si>
     <t>Messfehler Periodendauer in s</t>
@@ -112,6 +117,9 @@
   <si>
     <t>Phasenzeit in ms</t>
   </si>
+  <si>
+    <t>Eigenfrequenz in Hz</t>
+  </si>
 </sst>
 </file>
 
@@ -159,18 +167,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,6 +447,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Zeit in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -503,6 +564,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -552,6 +668,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -837,6 +984,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Zeit in s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -899,6 +1101,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -948,6 +1205,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1070,7 +1358,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1087,10 +1375,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1206,7 +1492,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C1AF-3149-9BB6-C88351A95C83}"/>
@@ -1246,6 +1532,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Anregungsfrequenz in (1/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1308,6 +1649,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1357,6 +1753,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1474,7 +1901,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1491,10 +1918,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1610,7 +2035,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-05DE-DF4C-AB91-1AF1106CC311}"/>
@@ -1650,6 +2075,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Anregungsfrequenz</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> in (1/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1712,6 +2197,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Phsenzeit</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1761,6 +2301,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -4034,15 +4605,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>8890</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>172720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4070,13 +4641,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>17780</xdr:colOff>
+      <xdr:colOff>10160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>16510</xdr:rowOff>
+      <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>782320</xdr:colOff>
+      <xdr:colOff>772160</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4113,8 +4684,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>386080</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4149,8 +4720,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4176,6 +4747,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4477,8 +5052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12BC500-A4FF-6045-ABAC-036A2B272161}">
   <dimension ref="B2:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4562,14 +5137,14 @@
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <f>SUM(D3:D7)/5</f>
         <v>1.9137999999999997</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
         <f>2*PI()/D8</f>
@@ -4578,27 +5153,27 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="2">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2">
         <f>ABS(-(2*PI())/(D8^2))*D11</f>
-        <v>5.1464531380727457E-2</v>
+        <v>0.10292906276145491</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
         <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
@@ -4606,7 +5181,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>B16*$D$42</f>
+        <f t="shared" ref="C16:C25" si="1">B16*$D$42</f>
         <v>0</v>
       </c>
       <c r="D16">
@@ -4618,14 +5193,14 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <f>B17*$D$42</f>
+        <f t="shared" si="1"/>
         <v>1.9460000000000002</v>
       </c>
       <c r="D17">
         <v>14.2</v>
       </c>
       <c r="L17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M17">
         <f>D17/D18</f>
@@ -4637,7 +5212,7 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <f>B18*$D$42</f>
+        <f t="shared" si="1"/>
         <v>3.8920000000000003</v>
       </c>
       <c r="D18">
@@ -4649,7 +5224,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <f>B19*$D$42</f>
+        <f t="shared" si="1"/>
         <v>5.838000000000001</v>
       </c>
       <c r="D19">
@@ -4661,7 +5236,7 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <f>B20*$D$42</f>
+        <f t="shared" si="1"/>
         <v>7.7840000000000007</v>
       </c>
       <c r="D20">
@@ -4673,7 +5248,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <f>B21*$D$42</f>
+        <f t="shared" si="1"/>
         <v>9.73</v>
       </c>
       <c r="D21">
@@ -4685,7 +5260,7 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <f>B22*$D$42</f>
+        <f t="shared" si="1"/>
         <v>11.676000000000002</v>
       </c>
       <c r="D22">
@@ -4697,7 +5272,7 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <f>B23*$D$42</f>
+        <f t="shared" si="1"/>
         <v>13.622000000000002</v>
       </c>
       <c r="D23">
@@ -4709,7 +5284,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <f>B24*$D$42</f>
+        <f t="shared" si="1"/>
         <v>15.568000000000001</v>
       </c>
       <c r="D24">
@@ -4721,7 +5296,7 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <f>B25*$D$42</f>
+        <f t="shared" si="1"/>
         <v>17.514000000000003</v>
       </c>
       <c r="D25">
@@ -4730,15 +5305,15 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
@@ -4746,7 +5321,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>B28*$D$39</f>
+        <f t="shared" ref="C28:C35" si="2">B28*$D$39</f>
         <v>0</v>
       </c>
       <c r="D28">
@@ -4758,14 +5333,14 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <f>B29*$D$39</f>
+        <f t="shared" si="2"/>
         <v>1.9449999999999998</v>
       </c>
       <c r="D29">
         <v>9.1999999999999993</v>
       </c>
       <c r="L29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M29">
         <f>D29/D30</f>
@@ -4777,7 +5352,7 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <f>B30*$D$39</f>
+        <f t="shared" si="2"/>
         <v>3.8899999999999997</v>
       </c>
       <c r="D30">
@@ -4789,7 +5364,7 @@
         <v>3</v>
       </c>
       <c r="C31">
-        <f>B31*$D$39</f>
+        <f t="shared" si="2"/>
         <v>5.8349999999999991</v>
       </c>
       <c r="D31">
@@ -4801,7 +5376,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <f>B32*$D$39</f>
+        <f t="shared" si="2"/>
         <v>7.7799999999999994</v>
       </c>
       <c r="D32">
@@ -4813,7 +5388,7 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <f>B33*$D$39</f>
+        <f t="shared" si="2"/>
         <v>9.7249999999999996</v>
       </c>
       <c r="D33">
@@ -4825,7 +5400,7 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <f>B34*$D$39</f>
+        <f t="shared" si="2"/>
         <v>11.669999999999998</v>
       </c>
       <c r="D34">
@@ -4837,7 +5412,7 @@
         <v>7</v>
       </c>
       <c r="C35">
-        <f>B35*$D$39</f>
+        <f t="shared" si="2"/>
         <v>13.614999999999998</v>
       </c>
       <c r="D35">
@@ -4845,31 +5420,31 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="I38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="I38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="5"/>
+      <c r="J38" s="6"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <f>SUM(D40:D41)</f>
         <v>1.9449999999999998</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J39">
         <v>0.27800000000000002</v>
@@ -4880,14 +5455,14 @@
         <v>0.93</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G40">
         <f>LN(M17)/D42</f>
         <v>8.6503245025290193E-2</v>
       </c>
       <c r="I40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J40">
         <f>LN(M29)/D39</f>
@@ -4901,7 +5476,7 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42">
         <f>SUM(D43:D44)</f>
@@ -4920,41 +5495,41 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" t="s">
         <v>22</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="I47" t="s">
         <v>18</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="7">
+      <c r="B48" s="4">
         <v>445</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="4">
         <v>1117</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="4">
         <v>1054</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="4">
         <f>C48+D48</f>
         <v>2171</v>
       </c>
@@ -4962,10 +5537,10 @@
         <f>2*PI()/E48*1000</f>
         <v>2.8941433934498324</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="5">
         <v>2.4</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="4">
         <v>65</v>
       </c>
       <c r="I48" s="1">
@@ -4974,350 +5549,350 @@
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="7">
+      <c r="B49" s="4">
         <v>465</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="4">
         <v>1058</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="4">
         <v>1026</v>
       </c>
-      <c r="E49" s="7">
-        <f t="shared" ref="E49:E60" si="1">C49+D49</f>
+      <c r="E49" s="4">
+        <f t="shared" ref="E49:E60" si="3">C49+D49</f>
         <v>2084</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" ref="F49:F60" si="2">2*PI()/E49*1000</f>
+        <f t="shared" ref="F49:F60" si="4">2*PI()/E49*1000</f>
         <v>3.0149641589153484</v>
       </c>
-      <c r="G49" s="8">
+      <c r="G49" s="5">
         <v>3.4</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="4">
         <v>122</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" ref="I49:I60" si="3">360*H49/E49</f>
+        <f t="shared" ref="I49:I60" si="5">360*H49/E49</f>
         <v>21.074856046065261</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B50" s="7">
+      <c r="B50" s="4">
         <v>475</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="4">
         <v>1034</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="4">
         <v>1015</v>
       </c>
-      <c r="E50" s="7">
-        <f t="shared" si="1"/>
+      <c r="E50" s="4">
+        <f t="shared" si="3"/>
         <v>2049</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.066464278760169</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="5">
         <v>4.5</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="4">
         <v>163</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>28.63836017569546</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B51" s="7">
+      <c r="B51" s="4">
         <v>485</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="4">
         <v>1001</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="4">
         <v>1003</v>
       </c>
-      <c r="E51" s="7">
-        <f t="shared" si="1"/>
+      <c r="E51" s="4">
+        <f t="shared" si="3"/>
         <v>2004</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.1353220095706518</v>
       </c>
-      <c r="G51" s="8">
+      <c r="G51" s="5">
         <v>6.4</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H51" s="4">
         <v>248</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>44.550898203592816</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B52" s="7">
+      <c r="B52" s="4">
         <v>490</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="4">
         <v>984</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="4">
         <v>998</v>
       </c>
-      <c r="E52" s="7">
-        <f t="shared" si="1"/>
+      <c r="E52" s="4">
+        <f t="shared" si="3"/>
         <v>1982</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.1701237674972682</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="5">
         <v>8</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52" s="4">
         <v>308</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>55.943491422805245</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="7">
+      <c r="B53" s="4">
         <v>495</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="4">
         <v>971</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="4">
         <v>994</v>
       </c>
-      <c r="E53" s="7">
-        <f t="shared" si="1"/>
+      <c r="E53" s="4">
+        <f t="shared" si="3"/>
         <v>1965</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.1975497746461001</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="5">
         <v>9.4</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H53" s="4">
         <v>397</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>72.732824427480921</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="7">
+      <c r="B54" s="4">
         <v>500</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="4">
         <v>959</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="4">
         <v>987</v>
       </c>
-      <c r="E54" s="7">
-        <f t="shared" si="1"/>
+      <c r="E54" s="4">
+        <f t="shared" si="3"/>
         <v>1946</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2287694281498389</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="5">
         <v>10</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H54" s="4">
         <v>498</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>92.127440904419316</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="7">
+      <c r="B55" s="4">
         <v>505</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="4">
         <v>950</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="4">
         <v>974</v>
       </c>
-      <c r="E55" s="7">
-        <f t="shared" si="1"/>
+      <c r="E55" s="4">
+        <f t="shared" si="3"/>
         <v>1924</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2656888290954194</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="5">
         <v>9.4</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H55" s="4">
         <v>617</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>115.44698544698545</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B56" s="7">
+      <c r="B56" s="4">
         <v>510</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="4">
         <v>946</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="4">
         <v>965</v>
       </c>
-      <c r="E56" s="7">
-        <f t="shared" si="1"/>
+      <c r="E56" s="4">
+        <f t="shared" si="3"/>
         <v>1911</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2879043993613744</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="5">
         <v>8.4</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56" s="4">
         <v>667</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>125.65149136577708</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B57" s="7">
+      <c r="B57" s="4">
         <v>515</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="4">
         <v>941</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="4">
         <v>950</v>
       </c>
-      <c r="E57" s="7">
-        <f t="shared" si="1"/>
+      <c r="E57" s="4">
+        <f t="shared" si="3"/>
         <v>1891</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.3226786394392311</v>
       </c>
-      <c r="G57" s="8">
+      <c r="G57" s="5">
         <v>7</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="4">
         <v>717</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>136.49920676890534</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B58" s="7">
+      <c r="B58" s="4">
         <v>525</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="4">
         <v>931</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="4">
         <v>924</v>
       </c>
-      <c r="E58" s="7">
-        <f t="shared" si="1"/>
+      <c r="E58" s="4">
+        <f t="shared" si="3"/>
         <v>1855</v>
       </c>
       <c r="F58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.3871618906628496</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="5">
         <v>4.8</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58" s="4">
         <v>761</v>
       </c>
       <c r="I58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>147.68733153638814</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B59" s="7">
+      <c r="B59" s="4">
         <v>535</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="4">
         <v>923</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="4">
         <v>901</v>
       </c>
-      <c r="E59" s="7">
-        <f t="shared" si="1"/>
+      <c r="E59" s="4">
+        <f t="shared" si="3"/>
         <v>1824</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.4447287868309138</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="5">
         <v>3.8</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="4">
         <v>777</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>153.35526315789474</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="7">
+      <c r="B60" s="4">
         <v>555</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="4">
         <v>906</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="4">
         <v>859</v>
       </c>
-      <c r="E60" s="7">
-        <f t="shared" si="1"/>
+      <c r="E60" s="4">
+        <f t="shared" si="3"/>
         <v>1765</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5598783610082645</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="5">
         <v>2.4</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60" s="4">
         <v>771</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>157.25779036827194</v>
       </c>
     </row>

</xml_diff>